<commit_message>
Correcting the time windows usage on constructive heuristic Start build a local search Correct some parts of real data input
</commit_message>
<xml_diff>
--- a/Real data input/Requests/Low 1/Requests.xlsx
+++ b/Real data input/Requests/Low 1/Requests.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3726D4AB-FBE2-4E64-89FF-4EBC913AAD4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797A5FDF-F812-4174-A400-BFF65CFDB9E1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="442">
   <si>
     <t>Passenger</t>
   </si>
@@ -1343,6 +1343,9 @@
   </si>
   <si>
     <t>NTU</t>
+  </si>
+  <si>
+    <t>22087E12</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1353,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1421,7 +1424,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="E259" sqref="E259:E884"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B260" sqref="B260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8271,8 +8274,8 @@
       <c r="A178" t="s">
         <v>201</v>
       </c>
-      <c r="B178" s="5">
-        <v>2.2087E+16</v>
+      <c r="B178" s="4" t="s">
+        <v>441</v>
       </c>
       <c r="C178" t="s">
         <v>12</v>
@@ -8530,8 +8533,8 @@
       <c r="A185" t="s">
         <v>31</v>
       </c>
-      <c r="B185" s="5">
-        <v>2.201E+92</v>
+      <c r="B185" s="4" t="s">
+        <v>424</v>
       </c>
       <c r="C185" t="s">
         <v>13</v>
@@ -11268,7 +11271,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B5 B23:B24 B28:B30 B91:B93 B196 B207" numberStoredAsText="1"/>
+    <ignoredError sqref="B5 B23:B24 B28:B30 B91:B93 B196 B207 B185 B178" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>